<commit_message>
Filled-in excel file add added register link in login
</commit_message>
<xml_diff>
--- a/Rendu-Projet-Complet.xlsx
+++ b/Rendu-Projet-Complet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\machaumont2\iut\dealabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\machaumont2\iut\dealabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3073EB-068D-4B46-9AB9-0F8BBA3CC9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF0677-1152-4FAF-9CEF-8A43E5944A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20448" windowHeight="11232" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20448" windowHeight="11232" activeTab="1" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
   </bookViews>
   <sheets>
     <sheet name="Partie 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Binome</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Non</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -278,111 +321,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -708,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F401AA-F8B3-C845-98CB-91317ACEBECA}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -774,7 +737,7 @@
     </row>
     <row r="8" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -782,7 +745,7 @@
     </row>
     <row r="9" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -790,7 +753,7 @@
     </row>
     <row r="10" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -822,7 +785,7 @@
     </row>
     <row r="14" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -830,7 +793,7 @@
     </row>
     <row r="15" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -854,7 +817,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -896,36 +859,28 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:C7 A19:A22 A8:A17">
-    <cfRule type="expression" dxfId="15" priority="7">
+  <conditionalFormatting sqref="A7:A22">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",A7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",A7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A22">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>"$A$7=Oui'"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>"$A$7 == 'NON'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:A22 A7:A17">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="11" priority="3">
+  <conditionalFormatting sqref="A7:C7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>"$A$7=Oui'"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>"$A$7 == 'NON'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -941,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995777F5-5494-3840-AC9A-36EDD3A31EBD}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -998,86 +953,123 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:C7 A8:A17">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>"$A$7=Oui'"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>"$A$7 == 'NON'"</formula>
+  <conditionalFormatting sqref="A7:A18">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",A7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",A7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:A17">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="A8:A18">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>"$A$7=Oui'"</formula>
     </cfRule>
@@ -1085,12 +1077,12 @@
       <formula>"$A$7 == 'NON'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Non">
-      <formula>NOT(ISERROR(SEARCH("Non",A18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",A18)))</formula>
+  <conditionalFormatting sqref="A7:C7">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>"$A$7=Oui'"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>"$A$7 == 'NON'"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>